<commit_message>
changed chr name format in enhancer bed
</commit_message>
<xml_diff>
--- a/data/Zhang_2020_HSPC_HiC_loops.xlsx
+++ b/data/Zhang_2020_HSPC_HiC_loops.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mira/Dropbox/HSPC Looping paper/Cell submission/0524 Figs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weihan/Desktop/Research/Jeff_project/CD34_HiC_CUX1_integration/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{883617C5-6E46-4D4A-9A05-239CFEFD9DE2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68176D4-00FB-D949-A388-925B84D77A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20280" yWindow="460" windowWidth="18120" windowHeight="22200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12740" yWindow="1160" windowWidth="25320" windowHeight="22200" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Long_loops" sheetId="1" r:id="rId1"/>
     <sheet name="HiCCUP_loops" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -91,12 +102,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -111,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -119,6 +142,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G410"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A188" workbookViewId="0">
-      <selection activeCell="H203" sqref="H203"/>
+    <sheetView showRuler="0" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47:F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9823,7 +9849,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G409">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G409">
     <sortCondition descending="1" ref="G2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9833,15 +9859,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G2684"/>
+  <dimension ref="A1:H2684"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A2667" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9864,7 +9890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -9887,7 +9913,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
@@ -9900,7 +9926,7 @@
       <c r="D3">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>99620000</v>
       </c>
       <c r="F3">
@@ -9910,30 +9936,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>16870000</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>16880000</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>17290000</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <v>17300000</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>10</v>
       </c>
@@ -9956,7 +9982,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10</v>
       </c>
@@ -9979,7 +10005,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>10</v>
       </c>
@@ -10002,7 +10028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>10</v>
       </c>
@@ -10025,7 +10051,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>10</v>
       </c>
@@ -10047,8 +10073,12 @@
       <c r="G9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <f>F9-E9</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -10071,7 +10101,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -10094,7 +10124,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -10117,7 +10147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -10140,7 +10170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -10163,7 +10193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>10</v>
       </c>
@@ -10186,7 +10216,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>10</v>
       </c>

</xml_diff>